<commit_message>
JH Erstellen von Objekt Unternehmen
</commit_message>
<xml_diff>
--- a/eingabe/Unternehmen.xlsx
+++ b/eingabe/Unternehmen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekt\eingabe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B30AEA21-4813-4259-9E86-7E60730CB190}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B83ED1-5BF2-4CF6-B6A9-60248D685B4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{3A9E2240-F68F-4045-AE50-B76F133D2F1C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Unternehmen</t>
   </si>
@@ -555,7 +555,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -707,7 +707,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -763,7 +763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -773,8 +773,11 @@
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -788,7 +791,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
JD: Tests fuer VorhandeneVeranstaltungen.java + kleinere Aenderungen in VorhandenenVeranstaltungen aus Gruenden der Testbarkeit
</commit_message>
<xml_diff>
--- a/eingabe/Unternehmen.xlsx
+++ b/eingabe/Unternehmen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekt\eingabe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84794F4F-9BB7-4C28-A28A-394A96441FD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655D4FD6-3D3A-465E-BC0B-876EA2E0BC8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{3A9E2240-F68F-4045-AE50-B76F133D2F1C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>Unternehmen</t>
   </si>
@@ -561,7 +561,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D28"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,15 +628,9 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -652,12 +646,8 @@
       <c r="D4" s="4">
         <v>20</v>
       </c>
-      <c r="E4" s="4">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -670,15 +660,11 @@
       <c r="C5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="4">
-        <v>20</v>
-      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4">
-        <v>5</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
JH: Ausgabe eines Raum und Zeitplans
</commit_message>
<xml_diff>
--- a/eingabe/Unternehmen.xlsx
+++ b/eingabe/Unternehmen.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>Unternehmen</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>Beamter im allgemeinen Vollzugsdienst, Dipl-Verwaltungswirt (FH)</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -560,11 +566,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6BCE577-6462-43C7-A707-99D40A5D160F}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection activeCell="F2" sqref="F2" activeCellId="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" defaultColWidth="11.42578125" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="1" bestFit="1" customWidth="1"/>
@@ -576,7 +582,7 @@
     <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -597,7 +603,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -611,14 +617,14 @@
         <v>20</v>
       </c>
       <c r="E2" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -633,7 +639,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -650,7 +656,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" ht="45">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -667,7 +673,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -688,7 +694,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -709,7 +715,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" ht="30">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -730,7 +736,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -751,7 +757,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -772,7 +778,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -793,7 +799,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -814,7 +820,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -835,7 +841,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -856,7 +862,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" ht="30">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -877,7 +883,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -898,7 +904,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -919,7 +925,7 @@
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" ht="30">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -940,7 +946,7 @@
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -961,7 +967,7 @@
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -982,7 +988,7 @@
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" ht="30">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1003,7 +1009,7 @@
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" ht="30">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1024,7 +1030,7 @@
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1045,7 +1051,7 @@
       </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1064,7 +1070,7 @@
       </c>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" ht="30">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1085,7 +1091,7 @@
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1104,7 +1110,7 @@
       </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1123,7 +1129,7 @@
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1142,25 +1148,25 @@
       </c>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32">
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34">
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35">
       <c r="G35" s="3"/>
     </row>
   </sheetData>

</xml_diff>